<commit_message>
Commit 07032018 at 3.20PM
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="9720" windowHeight="3660"/>
   </bookViews>
   <sheets>
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,10 +67,10 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>IE</t>
-  </si>
-  <si>
     <t>redmi note 4</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -380,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,7 +392,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +426,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -466,7 +467,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated script 0703 5.51PM
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -10,7 +10,6 @@
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,7 +69,7 @@
     <t>redmi note 4</t>
   </si>
   <si>
-    <t>IE</t>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -381,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -392,7 +391,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>